<commit_message>
una mejora para los mensajes
</commit_message>
<xml_diff>
--- a/CAADI_GROUPS/Maestria_3.xlsx
+++ b/CAADI_GROUPS/Maestria_3.xlsx
@@ -20,51 +20,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
-  <si>
-    <t xml:space="preserve">maestria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">englis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dorolfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zongalez</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+  <si>
+    <t xml:space="preserve">Maestría</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENGLISH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">José Ángel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calderón</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">angelcalderon2@hotmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosalba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pacheco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sanchez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rosspacheco90@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eduardo Miguel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">González</t>
   </si>
   <si>
     <t xml:space="preserve">García</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rosalba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pacheco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sanchez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rosspacheco90@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MIEA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eduardo Miguel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">González</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M</t>
   </si>
   <si>
     <t xml:space="preserve">em.gonzalezgarcia@ugto.mx</t>
@@ -105,7 +105,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -136,14 +136,6 @@
       <family val="0"/>
       <charset val="134"/>
     </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="134"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -190,36 +182,28 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -304,7 +288,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="A1:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -324,40 +308,39 @@
         <v>1</v>
       </c>
       <c r="C1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F2" s="1"/>
-      <c r="G2" s="2"/>
-    </row>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>146978</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="1" t="n">
+        <v>810069</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="4"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>146749</v>
       </c>
@@ -373,43 +356,43 @@
       <c r="E5" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="F5" s="3" t="n">
         <v>34301</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="n">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
         <v>736214</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="6" t="n">
+      <c r="F6" s="5" t="n">
         <v>32900</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>146734</v>
       </c>
@@ -423,19 +406,19 @@
         <v>19</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F7" s="3" t="n">
         <v>30683</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>146472</v>
       </c>
@@ -449,12 +432,12 @@
         <v>23</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F8" s="3" t="n">
         <v>33496</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="4" t="s">
         <v>24</v>
       </c>
       <c r="H8" s="0" t="s">
@@ -463,10 +446,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1" display="rosspacheco90@gmail.com"/>
-    <hyperlink ref="G6" r:id="rId2" display="em.gonzalezgarcia@ugto.mx"/>
-    <hyperlink ref="G7" r:id="rId3" display="elias.salazarmtz@gmail.com"/>
-    <hyperlink ref="G8" r:id="rId4" display="saos.pro12@gmail.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="angelcalderon2@hotmail.com"/>
+    <hyperlink ref="G5" r:id="rId2" display="rosspacheco90@gmail.com"/>
+    <hyperlink ref="G6" r:id="rId3" display="em.gonzalezgarcia@ugto.mx"/>
+    <hyperlink ref="G7" r:id="rId4" display="elias.salazarmtz@gmail.com"/>
+    <hyperlink ref="G8" r:id="rId5" display="saos.pro12@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>